<commit_message>
convert GSO data to CSV file
</commit_message>
<xml_diff>
--- a/data/raw/Weight/Ho_TBB01SR- ho trong lua 2020.xlsx
+++ b/data/raw/Weight/Ho_TBB01SR- ho trong lua 2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BThanh\SPIA Dropbox\SPIA General\SPIA 2019-2024\5. OBJ.3-Data collection\Country teams\Vietnam\DATA\Weight\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BThanh\Desktop\Viet-Nam-report-2024\data\raw\Weight\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5565E650-D771-4EF0-8D45-0C1E4210F1B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B6FAE9-F1E0-4BD4-91CE-A42118CB00D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1087,6 +1087,36 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1100,36 +1130,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1421,159 +1421,159 @@
       <selection pane="bottomLeft" activeCell="D4" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="0.69140625" style="25" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="0.69140625" style="26" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="27.15234375" customWidth="1"/>
-    <col min="5" max="5" width="13.53515625" customWidth="1"/>
-    <col min="6" max="6" width="13.53515625" style="39" customWidth="1"/>
-    <col min="7" max="8" width="13.53515625" customWidth="1"/>
-    <col min="9" max="9" width="13.53515625" style="65" customWidth="1"/>
-    <col min="10" max="15" width="13.53515625" customWidth="1"/>
-    <col min="16" max="16" width="13.53515625" style="49" customWidth="1"/>
-    <col min="17" max="35" width="13.53515625" customWidth="1"/>
-    <col min="36" max="36" width="13.53515625" style="56" customWidth="1"/>
-    <col min="37" max="37" width="13.53515625" customWidth="1"/>
-    <col min="38" max="38" width="13.53515625" style="56" customWidth="1"/>
-    <col min="39" max="43" width="13.53515625" customWidth="1"/>
-    <col min="44" max="44" width="9.15234375" style="7" customWidth="1"/>
-    <col min="45" max="16384" width="9.15234375" style="7"/>
+    <col min="1" max="2" width="0.7265625" style="25" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="0.7265625" style="26" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="27.1796875" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" style="39" customWidth="1"/>
+    <col min="7" max="8" width="13.54296875" customWidth="1"/>
+    <col min="9" max="9" width="13.54296875" style="65" customWidth="1"/>
+    <col min="10" max="15" width="13.54296875" customWidth="1"/>
+    <col min="16" max="16" width="13.54296875" style="49" customWidth="1"/>
+    <col min="17" max="35" width="13.54296875" customWidth="1"/>
+    <col min="36" max="36" width="13.54296875" style="56" customWidth="1"/>
+    <col min="37" max="37" width="13.54296875" customWidth="1"/>
+    <col min="38" max="38" width="13.54296875" style="56" customWidth="1"/>
+    <col min="39" max="43" width="13.54296875" customWidth="1"/>
+    <col min="44" max="44" width="9.1796875" style="7" customWidth="1"/>
+    <col min="45" max="16384" width="9.1796875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="D1" s="84" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
-      <c r="R1" s="84"/>
-      <c r="S1" s="84"/>
-      <c r="T1" s="84"/>
-      <c r="U1" s="84"/>
-      <c r="V1" s="84"/>
-      <c r="W1" s="84"/>
-      <c r="X1" s="84"/>
-      <c r="Y1" s="84"/>
-      <c r="Z1" s="84"/>
-      <c r="AA1" s="84"/>
-      <c r="AB1" s="84"/>
-      <c r="AC1" s="84"/>
-      <c r="AD1" s="84"/>
-      <c r="AE1" s="84"/>
-      <c r="AF1" s="84"/>
-      <c r="AG1" s="84"/>
-      <c r="AH1" s="84"/>
-      <c r="AI1" s="84"/>
-      <c r="AJ1" s="84"/>
-      <c r="AK1" s="84"/>
-      <c r="AL1" s="84"/>
-      <c r="AM1" s="84"/>
-      <c r="AN1" s="84"/>
-      <c r="AO1" s="84"/>
-      <c r="AP1" s="84"/>
-      <c r="AQ1" s="84"/>
-    </row>
-    <row r="2" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="D2" s="84" t="s">
+    <row r="1" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D1" s="77" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="77"/>
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
+      <c r="W1" s="77"/>
+      <c r="X1" s="77"/>
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="77"/>
+      <c r="AA1" s="77"/>
+      <c r="AB1" s="77"/>
+      <c r="AC1" s="77"/>
+      <c r="AD1" s="77"/>
+      <c r="AE1" s="77"/>
+      <c r="AF1" s="77"/>
+      <c r="AG1" s="77"/>
+      <c r="AH1" s="77"/>
+      <c r="AI1" s="77"/>
+      <c r="AJ1" s="77"/>
+      <c r="AK1" s="77"/>
+      <c r="AL1" s="77"/>
+      <c r="AM1" s="77"/>
+      <c r="AN1" s="77"/>
+      <c r="AO1" s="77"/>
+      <c r="AP1" s="77"/>
+      <c r="AQ1" s="77"/>
+    </row>
+    <row r="2" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D2" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84"/>
-      <c r="P2" s="84"/>
-      <c r="Q2" s="84"/>
-      <c r="R2" s="84"/>
-      <c r="S2" s="84"/>
-      <c r="T2" s="84"/>
-      <c r="U2" s="84"/>
-      <c r="V2" s="84"/>
-      <c r="W2" s="84"/>
-      <c r="X2" s="84"/>
-      <c r="Y2" s="84"/>
-      <c r="Z2" s="84"/>
-      <c r="AA2" s="84"/>
-      <c r="AB2" s="84"/>
-      <c r="AC2" s="84"/>
-      <c r="AD2" s="84"/>
-      <c r="AE2" s="84"/>
-      <c r="AF2" s="84"/>
-      <c r="AG2" s="84"/>
-      <c r="AH2" s="84"/>
-      <c r="AI2" s="84"/>
-      <c r="AJ2" s="84"/>
-      <c r="AK2" s="84"/>
-      <c r="AL2" s="84"/>
-      <c r="AM2" s="84"/>
-      <c r="AN2" s="84"/>
-      <c r="AO2" s="84"/>
-      <c r="AP2" s="84"/>
-      <c r="AQ2" s="84"/>
-    </row>
-    <row r="3" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="D3" s="85" t="s">
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
+      <c r="N2" s="77"/>
+      <c r="O2" s="77"/>
+      <c r="P2" s="77"/>
+      <c r="Q2" s="77"/>
+      <c r="R2" s="77"/>
+      <c r="S2" s="77"/>
+      <c r="T2" s="77"/>
+      <c r="U2" s="77"/>
+      <c r="V2" s="77"/>
+      <c r="W2" s="77"/>
+      <c r="X2" s="77"/>
+      <c r="Y2" s="77"/>
+      <c r="Z2" s="77"/>
+      <c r="AA2" s="77"/>
+      <c r="AB2" s="77"/>
+      <c r="AC2" s="77"/>
+      <c r="AD2" s="77"/>
+      <c r="AE2" s="77"/>
+      <c r="AF2" s="77"/>
+      <c r="AG2" s="77"/>
+      <c r="AH2" s="77"/>
+      <c r="AI2" s="77"/>
+      <c r="AJ2" s="77"/>
+      <c r="AK2" s="77"/>
+      <c r="AL2" s="77"/>
+      <c r="AM2" s="77"/>
+      <c r="AN2" s="77"/>
+      <c r="AO2" s="77"/>
+      <c r="AP2" s="77"/>
+      <c r="AQ2" s="77"/>
+    </row>
+    <row r="3" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D3" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
-      <c r="O3" s="85"/>
-      <c r="P3" s="85"/>
-      <c r="Q3" s="85"/>
-      <c r="R3" s="85"/>
-      <c r="S3" s="85"/>
-      <c r="T3" s="85"/>
-      <c r="U3" s="85"/>
-      <c r="V3" s="85"/>
-      <c r="W3" s="85"/>
-      <c r="X3" s="85"/>
-      <c r="Y3" s="85"/>
-      <c r="Z3" s="85"/>
-      <c r="AA3" s="85"/>
-      <c r="AB3" s="85"/>
-      <c r="AC3" s="85"/>
-      <c r="AD3" s="85"/>
-      <c r="AE3" s="85"/>
-      <c r="AF3" s="85"/>
-      <c r="AG3" s="85"/>
-      <c r="AH3" s="85"/>
-      <c r="AI3" s="85"/>
-      <c r="AJ3" s="85"/>
-      <c r="AK3" s="85"/>
-      <c r="AL3" s="85"/>
-      <c r="AM3" s="85"/>
-      <c r="AN3" s="85"/>
-      <c r="AO3" s="85"/>
-      <c r="AP3" s="85"/>
-      <c r="AQ3" s="85"/>
-    </row>
-    <row r="4" spans="1:43" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="78"/>
+      <c r="K3" s="78"/>
+      <c r="L3" s="78"/>
+      <c r="M3" s="78"/>
+      <c r="N3" s="78"/>
+      <c r="O3" s="78"/>
+      <c r="P3" s="78"/>
+      <c r="Q3" s="78"/>
+      <c r="R3" s="78"/>
+      <c r="S3" s="78"/>
+      <c r="T3" s="78"/>
+      <c r="U3" s="78"/>
+      <c r="V3" s="78"/>
+      <c r="W3" s="78"/>
+      <c r="X3" s="78"/>
+      <c r="Y3" s="78"/>
+      <c r="Z3" s="78"/>
+      <c r="AA3" s="78"/>
+      <c r="AB3" s="78"/>
+      <c r="AC3" s="78"/>
+      <c r="AD3" s="78"/>
+      <c r="AE3" s="78"/>
+      <c r="AF3" s="78"/>
+      <c r="AG3" s="78"/>
+      <c r="AH3" s="78"/>
+      <c r="AI3" s="78"/>
+      <c r="AJ3" s="78"/>
+      <c r="AK3" s="78"/>
+      <c r="AL3" s="78"/>
+      <c r="AM3" s="78"/>
+      <c r="AN3" s="78"/>
+      <c r="AO3" s="78"/>
+      <c r="AP3" s="78"/>
+      <c r="AQ3" s="78"/>
+    </row>
+    <row r="4" spans="1:43" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
       <c r="C4" s="13"/>
@@ -1615,25 +1615,25 @@
       <c r="AM4" s="5"/>
       <c r="AN4" s="5"/>
       <c r="AO4" s="5"/>
-      <c r="AP4" s="79" t="s">
+      <c r="AP4" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="AQ4" s="79"/>
-    </row>
-    <row r="5" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="83" t="s">
+      <c r="AQ4" s="89"/>
+    </row>
+    <row r="5" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="83" t="s">
+      <c r="B5" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="82" t="s">
+      <c r="C5" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="81" t="s">
+      <c r="D5" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="81" t="s">
+      <c r="E5" s="79" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="80" t="s">
@@ -1677,26 +1677,26 @@
       <c r="AP5" s="80"/>
       <c r="AQ5" s="80"/>
     </row>
-    <row r="6" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="83"/>
-      <c r="B6" s="83"/>
-      <c r="C6" s="82"/>
-      <c r="D6" s="81"/>
-      <c r="E6" s="81"/>
-      <c r="F6" s="89" t="s">
+    <row r="6" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="76"/>
+      <c r="B6" s="76"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="79"/>
+      <c r="E6" s="79"/>
+      <c r="F6" s="84" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="75" t="s">
+      <c r="G6" s="85" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="76" t="s">
+      <c r="H6" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="77"/>
-      <c r="J6" s="77"/>
-      <c r="K6" s="77"/>
-      <c r="L6" s="78"/>
-      <c r="M6" s="81" t="s">
+      <c r="I6" s="87"/>
+      <c r="J6" s="87"/>
+      <c r="K6" s="87"/>
+      <c r="L6" s="88"/>
+      <c r="M6" s="79" t="s">
         <v>13</v>
       </c>
       <c r="N6" s="80" t="s">
@@ -1714,21 +1714,21 @@
       <c r="X6" s="80"/>
       <c r="Y6" s="80"/>
       <c r="Z6" s="80"/>
-      <c r="AA6" s="81" t="s">
+      <c r="AA6" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="AB6" s="86" t="s">
+      <c r="AB6" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="AC6" s="87"/>
-      <c r="AD6" s="87"/>
-      <c r="AE6" s="87"/>
-      <c r="AF6" s="87"/>
-      <c r="AG6" s="88"/>
-      <c r="AH6" s="81" t="s">
+      <c r="AC6" s="82"/>
+      <c r="AD6" s="82"/>
+      <c r="AE6" s="82"/>
+      <c r="AF6" s="82"/>
+      <c r="AG6" s="83"/>
+      <c r="AH6" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="AI6" s="81" t="s">
+      <c r="AI6" s="79" t="s">
         <v>16</v>
       </c>
       <c r="AJ6" s="80" t="s">
@@ -1740,18 +1740,18 @@
       <c r="AN6" s="80"/>
       <c r="AO6" s="80"/>
       <c r="AP6" s="80"/>
-      <c r="AQ6" s="81" t="s">
+      <c r="AQ6" s="79" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:43" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="83"/>
-      <c r="B7" s="83"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="81"/>
-      <c r="E7" s="81"/>
-      <c r="F7" s="89"/>
-      <c r="G7" s="75"/>
+    <row r="7" spans="1:43" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="76"/>
+      <c r="B7" s="76"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="79"/>
+      <c r="F7" s="84"/>
+      <c r="G7" s="85"/>
       <c r="H7" s="1" t="s">
         <v>18</v>
       </c>
@@ -1767,7 +1767,7 @@
       <c r="L7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M7" s="81"/>
+      <c r="M7" s="79"/>
       <c r="N7" s="1" t="s">
         <v>22</v>
       </c>
@@ -1807,7 +1807,7 @@
       <c r="Z7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AA7" s="81"/>
+      <c r="AA7" s="79"/>
       <c r="AB7" s="1" t="s">
         <v>35</v>
       </c>
@@ -1826,8 +1826,8 @@
       <c r="AG7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AH7" s="81"/>
-      <c r="AI7" s="81"/>
+      <c r="AH7" s="79"/>
+      <c r="AI7" s="79"/>
       <c r="AJ7" s="51" t="s">
         <v>41</v>
       </c>
@@ -1849,9 +1849,9 @@
       <c r="AP7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AQ7" s="81"/>
-    </row>
-    <row r="8" spans="1:43" s="74" customFormat="1" ht="25.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AQ7" s="79"/>
+    </row>
+    <row r="8" spans="1:43" s="74" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="66"/>
       <c r="B8" s="66"/>
       <c r="C8" s="67"/>
@@ -1966,7 +1966,7 @@
       </c>
       <c r="AQ8" s="68"/>
     </row>
-    <row r="9" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="14"/>
       <c r="B9" s="14"/>
       <c r="C9" s="15"/>
@@ -2091,7 +2091,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:43" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:43" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
       <c r="C10" s="18"/>
@@ -2216,7 +2216,7 @@
         <v>98591.060343861594</v>
       </c>
     </row>
-    <row r="11" spans="1:43" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:43" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="17">
         <v>1</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>13564.003664731999</v>
       </c>
     </row>
-    <row r="12" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9">
         <v>1</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>984.60070610046398</v>
       </c>
     </row>
-    <row r="13" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9">
         <v>1</v>
       </c>
@@ -2601,7 +2601,7 @@
         <v>360.861083984375</v>
       </c>
     </row>
-    <row r="14" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="9">
         <v>1</v>
       </c>
@@ -2730,7 +2730,7 @@
         <v>374.50480985641502</v>
       </c>
     </row>
-    <row r="15" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9">
         <v>1</v>
       </c>
@@ -2859,7 +2859,7 @@
         <v>1458.74099063873</v>
       </c>
     </row>
-    <row r="16" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9">
         <v>1</v>
       </c>
@@ -2988,7 +2988,7 @@
         <v>4623.3450365066501</v>
       </c>
     </row>
-    <row r="17" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="9">
         <v>1</v>
       </c>
@@ -3117,7 +3117,7 @@
         <v>1114.6633865833301</v>
       </c>
     </row>
-    <row r="18" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="9">
         <v>1</v>
       </c>
@@ -3246,7 +3246,7 @@
         <v>229.66047716140699</v>
       </c>
     </row>
-    <row r="19" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9">
         <v>1</v>
       </c>
@@ -3375,7 +3375,7 @@
         <v>1508.5036387443499</v>
       </c>
     </row>
-    <row r="20" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9">
         <v>1</v>
       </c>
@@ -3504,7 +3504,7 @@
         <v>210.87369871139501</v>
       </c>
     </row>
-    <row r="21" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="9">
         <v>1</v>
       </c>
@@ -3633,7 +3633,7 @@
         <v>1850.22902202606</v>
       </c>
     </row>
-    <row r="22" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="9">
         <v>1</v>
       </c>
@@ -3762,7 +3762,7 @@
         <v>848.02081441879295</v>
       </c>
     </row>
-    <row r="23" spans="1:43" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:43" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="17">
         <v>2</v>
       </c>
@@ -3889,7 +3889,7 @@
         <v>3178.56330525875</v>
       </c>
     </row>
-    <row r="24" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="9">
         <v>2</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>53.456840038299603</v>
       </c>
     </row>
-    <row r="25" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="9">
         <v>2</v>
       </c>
@@ -4147,7 +4147,7 @@
         <v>14.257962942123401</v>
       </c>
     </row>
-    <row r="26" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="9">
         <v>2</v>
       </c>
@@ -4276,7 +4276,7 @@
         <v>11.9123425483704</v>
       </c>
     </row>
-    <row r="27" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="9">
         <v>2</v>
       </c>
@@ -4405,7 +4405,7 @@
         <v>200.395398616791</v>
       </c>
     </row>
-    <row r="28" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="9">
         <v>2</v>
       </c>
@@ -4534,7 +4534,7 @@
         <v>32.794224262237499</v>
       </c>
     </row>
-    <row r="29" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="9">
         <v>2</v>
       </c>
@@ -4663,7 +4663,7 @@
         <v>1019.21977567673</v>
       </c>
     </row>
-    <row r="30" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="9">
         <v>2</v>
       </c>
@@ -4792,7 +4792,7 @@
         <v>200.98623371124299</v>
       </c>
     </row>
-    <row r="31" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="9">
         <v>2</v>
       </c>
@@ -4921,7 +4921,7 @@
         <v>44.272666931152301</v>
       </c>
     </row>
-    <row r="32" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="9">
         <v>2</v>
       </c>
@@ -5050,7 +5050,7 @@
         <v>110.73059511184699</v>
       </c>
     </row>
-    <row r="33" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="9">
         <v>2</v>
       </c>
@@ -5179,7 +5179,7 @@
         <v>227.55393588542901</v>
       </c>
     </row>
-    <row r="34" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="9">
         <v>2</v>
       </c>
@@ -5308,7 +5308,7 @@
         <v>25.742919921875</v>
       </c>
     </row>
-    <row r="35" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="9">
         <v>2</v>
       </c>
@@ -5437,7 +5437,7 @@
         <v>360.291159629822</v>
       </c>
     </row>
-    <row r="36" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="9">
         <v>2</v>
       </c>
@@ -5566,7 +5566,7 @@
         <v>637.51729631423996</v>
       </c>
     </row>
-    <row r="37" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="9">
         <v>2</v>
       </c>
@@ -5695,7 +5695,7 @@
         <v>239.43195366859399</v>
       </c>
     </row>
-    <row r="38" spans="1:43" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:43" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="17">
         <v>3</v>
       </c>
@@ -5822,7 +5822,7 @@
         <v>34826.471759319298</v>
       </c>
     </row>
-    <row r="39" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="9">
         <v>3</v>
       </c>
@@ -5951,7 +5951,7 @@
         <v>3117.9489812851002</v>
       </c>
     </row>
-    <row r="40" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="9">
         <v>3</v>
       </c>
@@ -6080,7 +6080,7 @@
         <v>1744.27018404007</v>
       </c>
     </row>
-    <row r="41" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="9">
         <v>3</v>
       </c>
@@ -6209,7 +6209,7 @@
         <v>3035.41285681725</v>
       </c>
     </row>
-    <row r="42" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="9">
         <v>3</v>
       </c>
@@ -6338,7 +6338,7 @@
         <v>4304.8594965934799</v>
       </c>
     </row>
-    <row r="43" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="9">
         <v>3</v>
       </c>
@@ -6467,7 +6467,7 @@
         <v>1320.2966463565799</v>
       </c>
     </row>
-    <row r="44" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="9">
         <v>3</v>
       </c>
@@ -6596,7 +6596,7 @@
         <v>4605.1225116252899</v>
       </c>
     </row>
-    <row r="45" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="9">
         <v>3</v>
       </c>
@@ -6725,7 +6725,7 @@
         <v>281.20867848396301</v>
       </c>
     </row>
-    <row r="46" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="9">
         <v>3</v>
       </c>
@@ -6854,7 +6854,7 @@
         <v>2179.25538063049</v>
       </c>
     </row>
-    <row r="47" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="9">
         <v>3</v>
       </c>
@@ -6983,7 +6983,7 @@
         <v>1878.8850207328801</v>
       </c>
     </row>
-    <row r="48" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="9">
         <v>3</v>
       </c>
@@ -7112,7 +7112,7 @@
         <v>4253.70506286621</v>
       </c>
     </row>
-    <row r="49" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="9">
         <v>3</v>
       </c>
@@ -7241,7 +7241,7 @@
         <v>2427.1964735984802</v>
       </c>
     </row>
-    <row r="50" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="9">
         <v>3</v>
       </c>
@@ -7370,7 +7370,7 @@
         <v>4553.8383278846704</v>
       </c>
     </row>
-    <row r="51" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="9">
         <v>3</v>
       </c>
@@ -7499,7 +7499,7 @@
         <v>922.07396793365501</v>
       </c>
     </row>
-    <row r="52" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="9">
         <v>3</v>
       </c>
@@ -7628,7 +7628,7 @@
         <v>202.39817047119101</v>
       </c>
     </row>
-    <row r="53" spans="1:43" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:43" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="17">
         <v>4</v>
       </c>
@@ -7755,7 +7755,7 @@
         <v>678.52790021896396</v>
       </c>
     </row>
-    <row r="54" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="9">
         <v>4</v>
       </c>
@@ -7884,7 +7884,7 @@
         <v>79.064799785613999</v>
       </c>
     </row>
-    <row r="55" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="9">
         <v>4</v>
       </c>
@@ -8013,7 +8013,7 @@
         <v>153.082636833191</v>
       </c>
     </row>
-    <row r="56" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A56" s="9">
         <v>4</v>
       </c>
@@ -8142,7 +8142,7 @@
         <v>410.87198925018299</v>
       </c>
     </row>
-    <row r="57" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="9">
         <v>4</v>
       </c>
@@ -8271,7 +8271,7 @@
         <v>23.370940208435101</v>
       </c>
     </row>
-    <row r="58" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="9">
         <v>4</v>
       </c>
@@ -8400,7 +8400,7 @@
         <v>12.137534141540501</v>
       </c>
     </row>
-    <row r="59" spans="1:43" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:43" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A59" s="17">
         <v>5</v>
       </c>
@@ -8527,7 +8527,7 @@
         <v>6321.8266315460196</v>
       </c>
     </row>
-    <row r="60" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A60" s="9">
         <v>5</v>
       </c>
@@ -8656,7 +8656,7 @@
         <v>141.753993988037</v>
       </c>
     </row>
-    <row r="61" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A61" s="9">
         <v>5</v>
       </c>
@@ -8785,7 +8785,7 @@
         <v>2332.3723640441899</v>
       </c>
     </row>
-    <row r="62" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="9">
         <v>5</v>
       </c>
@@ -8914,7 +8914,7 @@
         <v>67.783110857009902</v>
       </c>
     </row>
-    <row r="63" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A63" s="9">
         <v>5</v>
       </c>
@@ -9043,7 +9043,7 @@
         <v>2187.0528345108</v>
       </c>
     </row>
-    <row r="64" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="9">
         <v>5</v>
       </c>
@@ -9172,7 +9172,7 @@
         <v>1148.8802411556201</v>
       </c>
     </row>
-    <row r="65" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A65" s="9">
         <v>5</v>
       </c>
@@ -9301,7 +9301,7 @@
         <v>443.98408699035599</v>
       </c>
     </row>
-    <row r="66" spans="1:43" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:43" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A66" s="17">
         <v>6</v>
       </c>
@@ -9428,7 +9428,7 @@
         <v>40021.667082786596</v>
       </c>
     </row>
-    <row r="67" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A67" s="9">
         <v>6</v>
       </c>
@@ -9557,7 +9557,7 @@
         <v>995.27333402633701</v>
       </c>
     </row>
-    <row r="68" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A68" s="9">
         <v>6</v>
       </c>
@@ -9686,7 +9686,7 @@
         <v>1622.6040070056899</v>
       </c>
     </row>
-    <row r="69" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A69" s="9">
         <v>6</v>
       </c>
@@ -9815,7 +9815,7 @@
         <v>5945.5674138069198</v>
       </c>
     </row>
-    <row r="70" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A70" s="9">
         <v>6</v>
       </c>
@@ -9944,7 +9944,7 @@
         <v>1536.9355928897901</v>
       </c>
     </row>
-    <row r="71" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A71" s="9">
         <v>6</v>
       </c>
@@ -10073,7 +10073,7 @@
         <v>541.55449795722996</v>
       </c>
     </row>
-    <row r="72" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A72" s="9">
         <v>6</v>
       </c>
@@ -10202,7 +10202,7 @@
         <v>2836.2106084823599</v>
       </c>
     </row>
-    <row r="73" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A73" s="9">
         <v>6</v>
       </c>
@@ -10331,7 +10331,7 @@
         <v>7124.9199156761197</v>
       </c>
     </row>
-    <row r="74" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A74" s="9">
         <v>6</v>
       </c>
@@ -10460,7 +10460,7 @@
         <v>7939.5926666259802</v>
       </c>
     </row>
-    <row r="75" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A75" s="9">
         <v>6</v>
       </c>
@@ -10589,7 +10589,7 @@
         <v>1109.5779685974101</v>
       </c>
     </row>
-    <row r="76" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A76" s="9">
         <v>6</v>
       </c>
@@ -10718,7 +10718,7 @@
         <v>629.86654710769699</v>
       </c>
     </row>
-    <row r="77" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A77" s="9">
         <v>6</v>
       </c>
@@ -10847,7 +10847,7 @@
         <v>1727.89770317078</v>
       </c>
     </row>
-    <row r="78" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A78" s="9">
         <v>6</v>
       </c>
@@ -10976,7 +10976,7 @@
         <v>3693.48230457306</v>
       </c>
     </row>
-    <row r="79" spans="1:43" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A79" s="21">
         <v>6</v>
       </c>
@@ -11107,6 +11107,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:L6"/>
+    <mergeCell ref="AP4:AQ4"/>
+    <mergeCell ref="AJ6:AP6"/>
+    <mergeCell ref="AQ6:AQ7"/>
     <mergeCell ref="C5:C7"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="D1:AQ1"/>
@@ -11123,11 +11128,6 @@
     <mergeCell ref="E5:E7"/>
     <mergeCell ref="F5:AQ5"/>
     <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="AP4:AQ4"/>
-    <mergeCell ref="AJ6:AP6"/>
-    <mergeCell ref="AQ6:AQ7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11139,23 +11139,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E713C3B-2AFB-4A24-98D1-6DA1C22259D1}">
   <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.4609375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.53515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.53515625" customWidth="1"/>
-    <col min="5" max="5" width="12.4609375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.53515625" style="33" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.54296875" style="33" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="39" t="s">
         <v>161</v>
       </c>
       <c r="B1">
@@ -11174,7 +11172,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
         <v>88</v>
       </c>
@@ -11195,7 +11193,7 @@
       </c>
       <c r="G2" s="33"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>89</v>
       </c>
@@ -11215,7 +11213,7 @@
         <v>2208822.2452724124</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
         <v>90</v>
       </c>
@@ -11237,7 +11235,7 @@
         <v>475243.62933219899</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>91</v>
       </c>
@@ -11259,7 +11257,7 @@
         <v>147854.9061435906</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>92</v>
       </c>
@@ -11281,7 +11279,7 @@
         <v>169886.94781581001</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>93</v>
       </c>
@@ -11303,7 +11301,7 @@
         <v>79166.201748384497</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
         <v>94</v>
       </c>
@@ -11323,7 +11321,7 @@
         <v>222982.6932737882</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
         <v>95</v>
       </c>
@@ -11345,7 +11343,7 @@
         <v>141507.0289965836</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>96</v>
       </c>
@@ -11367,7 +11365,7 @@
         <v>98142.687796522121</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
         <v>97</v>
       </c>
@@ -11389,7 +11387,7 @@
         <v>341677.33764278656</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
         <v>98</v>
       </c>
@@ -11411,7 +11409,7 @@
         <v>132285.00299412466</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
         <v>99</v>
       </c>
@@ -11433,7 +11431,7 @@
         <v>260936.54876480423</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
         <v>100</v>
       </c>
@@ -11455,7 +11453,7 @@
         <v>143822.92340977158</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
         <v>101</v>
       </c>
@@ -11475,7 +11473,7 @@
         <v>1802645.8789059676</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
         <v>102</v>
       </c>
@@ -11495,7 +11493,7 @@
         <v>112547.76490216691</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
         <v>103</v>
       </c>
@@ -11515,7 +11513,7 @@
         <v>73095.875843245347</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
         <v>104</v>
       </c>
@@ -11535,7 +11533,7 @@
         <v>53304.381461276629</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
         <v>105</v>
       </c>
@@ -11555,7 +11553,7 @@
         <v>126105.84918108153</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
         <v>106</v>
       </c>
@@ -11575,7 +11573,7 @@
         <v>89334.367479895373</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
         <v>107</v>
       </c>
@@ -11595,7 +11593,7 @@
         <v>122507.70251878598</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
         <v>108</v>
       </c>
@@ -11615,7 +11613,7 @@
         <v>151274.27679470397</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">
         <v>109</v>
       </c>
@@ -11635,7 +11633,7 @@
         <v>139679.69560507764</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="11" t="s">
         <v>110</v>
       </c>
@@ -11657,7 +11655,7 @@
         <v>297686.42153641651</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
         <v>111</v>
       </c>
@@ -11679,7 +11677,7 @@
         <v>188082.58031216878</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
         <v>112</v>
       </c>
@@ -11699,7 +11697,7 @@
         <v>96730.637949012671</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="11" t="s">
         <v>113</v>
       </c>
@@ -11719,7 +11717,7 @@
         <v>73857.550156367637</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="11" t="s">
         <v>114</v>
       </c>
@@ -11739,7 +11737,7 @@
         <v>162766.28867117915</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="11" t="s">
         <v>115</v>
       </c>
@@ -11759,7 +11757,7 @@
         <v>118955.49475239473</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="19" t="s">
         <v>116</v>
       </c>
@@ -11779,7 +11777,7 @@
         <v>2286617.6898868792</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="11" t="s">
         <v>117</v>
       </c>
@@ -11801,7 +11799,7 @@
         <v>548344.16468268202</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="11" t="s">
         <v>118</v>
       </c>
@@ -11823,7 +11821,7 @@
         <v>463261.91930899111</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="11" t="s">
         <v>119</v>
       </c>
@@ -11845,7 +11843,7 @@
         <v>178758.25121531688</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="11" t="s">
         <v>120</v>
       </c>
@@ -11867,7 +11865,7 @@
         <v>110231.83942243982</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="11" t="s">
         <v>121</v>
       </c>
@@ -11889,7 +11887,7 @@
         <v>66697.635799681433</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="11" t="s">
         <v>122</v>
       </c>
@@ -11911,7 +11909,7 @@
         <v>76216.014416420832</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="11" t="s">
         <v>123</v>
       </c>
@@ -11933,7 +11931,7 @@
         <v>12550.690909448793</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="11" t="s">
         <v>124</v>
       </c>
@@ -11955,7 +11953,7 @@
         <v>239731.13296428876</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="11" t="s">
         <v>125</v>
       </c>
@@ -11977,7 +11975,7 @@
         <v>153133.18652784143</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="11" t="s">
         <v>126</v>
       </c>
@@ -11999,7 +11997,7 @@
         <v>200279.27353955552</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="11" t="s">
         <v>127</v>
       </c>
@@ -12021,7 +12019,7 @@
         <v>109803.36561673712</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="11" t="s">
         <v>128</v>
       </c>
@@ -12043,7 +12041,7 @@
         <v>49690.503738534309</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="11" t="s">
         <v>129</v>
       </c>
@@ -12065,7 +12063,7 @@
         <v>26846.268226873312</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="11" t="s">
         <v>130</v>
       </c>
@@ -12087,7 +12085,7 @@
         <v>53553.535172419295</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="19" t="s">
         <v>131</v>
       </c>
@@ -12107,7 +12105,7 @@
         <v>411228.3781573333</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="11" t="s">
         <v>132</v>
       </c>
@@ -12127,7 +12125,7 @@
         <v>56126.60822672124</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="11" t="s">
         <v>133</v>
       </c>
@@ -12149,7 +12147,7 @@
         <v>144096.50151949539</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="11" t="s">
         <v>134</v>
       </c>
@@ -12171,7 +12169,7 @@
         <v>162932.37947201764</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="11" t="s">
         <v>135</v>
       </c>
@@ -12191,7 +12189,7 @@
         <v>22259.269688568209</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="11" t="s">
         <v>136</v>
       </c>
@@ -12211,7 +12209,7 @@
         <v>26943.633555835659</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="19" t="s">
         <v>137</v>
       </c>
@@ -12231,7 +12229,7 @@
         <v>79997.085776657274</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="11" t="s">
         <v>138</v>
       </c>
@@ -12251,7 +12249,7 @@
         <v>8912.3669354011272</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="11" t="s">
         <v>139</v>
       </c>
@@ -12271,7 +12269,7 @@
         <v>30042.119126152535</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="11" t="s">
         <v>140</v>
       </c>
@@ -12291,7 +12289,7 @@
         <v>1080.2596289040671</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="11" t="s">
         <v>141</v>
       </c>
@@ -12311,7 +12309,7 @@
         <v>22359.072447065872</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="11" t="s">
         <v>142</v>
       </c>
@@ -12331,7 +12329,7 @@
         <v>6830.1231371901804</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" s="11" t="s">
         <v>143</v>
       </c>
@@ -12351,7 +12349,7 @@
         <v>11645.233265834961</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" s="19" t="s">
         <v>144</v>
       </c>
@@ -12371,7 +12369,7 @@
         <v>942520.23839908384</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" s="11" t="s">
         <v>145</v>
       </c>
@@ -12393,7 +12391,7 @@
         <v>90333.152760497862</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" s="11" t="s">
         <v>146</v>
       </c>
@@ -12415,7 +12413,7 @@
         <v>55231.971749266384</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="11" t="s">
         <v>147</v>
       </c>
@@ -12437,7 +12435,7 @@
         <v>16726.301287840724</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" s="11" t="s">
         <v>148</v>
       </c>
@@ -12459,7 +12457,7 @@
         <v>63585.000484952223</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="11" t="s">
         <v>149</v>
       </c>
@@ -12481,7 +12479,7 @@
         <v>55127.509363538047</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" s="11" t="s">
         <v>150</v>
       </c>
@@ -12503,7 +12501,7 @@
         <v>89894.382250779119</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="11" t="s">
         <v>151</v>
       </c>
@@ -12525,7 +12523,7 @@
         <v>114017.66509568963</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" s="11" t="s">
         <v>152</v>
       </c>
@@ -12547,7 +12545,7 @@
         <v>198409.77945208017</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" s="11" t="s">
         <v>153</v>
       </c>
@@ -12569,7 +12567,7 @@
         <v>37518.666782105327</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" s="11" t="s">
         <v>154</v>
       </c>
@@ -12591,7 +12589,7 @@
         <v>55826.709730412971</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" s="11" t="s">
         <v>155</v>
       </c>
@@ -12613,7 +12611,7 @@
         <v>70202.801863033295</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" s="11" t="s">
         <v>156</v>
       </c>
@@ -12635,7 +12633,7 @@
         <v>78922.596797967446</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" s="23" t="s">
         <v>157</v>
       </c>
@@ -12657,7 +12655,7 @@
         <v>42562.858872142016</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" s="40" t="s">
         <v>162</v>
       </c>
@@ -12683,16 +12681,16 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.84375" customWidth="1"/>
-    <col min="2" max="2" width="13.69140625" customWidth="1"/>
-    <col min="3" max="3" width="12.3828125" customWidth="1"/>
-    <col min="4" max="4" width="12.53515625" customWidth="1"/>
-    <col min="5" max="5" width="11.53515625" customWidth="1"/>
+    <col min="1" max="1" width="33.81640625" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" customWidth="1"/>
+    <col min="3" max="3" width="12.36328125" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24.9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>198</v>
       </c>
@@ -12709,7 +12707,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
         <v>199</v>
       </c>
@@ -12732,7 +12730,7 @@
         <v>508884.68725794402</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>89</v>
       </c>
@@ -12740,7 +12738,7 @@
         <v>31834.800645112999</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
         <v>90</v>
       </c>
@@ -12748,7 +12746,7 @@
         <v>7658.2882795333899</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>91</v>
       </c>
@@ -12756,7 +12754,7 @@
         <v>10137.058778762799</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>92</v>
       </c>
@@ -12764,7 +12762,7 @@
         <v>814.90618515014603</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>93</v>
       </c>
@@ -12772,7 +12770,7 @@
         <v>1191.8886818885801</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
         <v>94</v>
       </c>
@@ -12780,7 +12778,7 @@
         <v>4724.30898547173</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
         <v>95</v>
       </c>
@@ -12788,7 +12786,7 @@
         <v>617.90470218658402</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>96</v>
       </c>
@@ -12796,7 +12794,7 @@
         <v>538.96769905090298</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
         <v>97</v>
       </c>
@@ -12804,7 +12802,7 @@
         <v>2539.80978965759</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
         <v>98</v>
       </c>
@@ -12812,7 +12810,7 @@
         <v>242.40541362762499</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
         <v>99</v>
       </c>
@@ -12820,7 +12818,7 @@
         <v>1383.80921936035</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
         <v>100</v>
       </c>
@@ -12828,7 +12826,7 @@
         <v>1985.4529104232799</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
         <v>101</v>
       </c>
@@ -12836,7 +12834,7 @@
         <v>247555.41617059699</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
         <v>102</v>
       </c>
@@ -12844,7 +12842,7 @@
         <v>31800.831166982702</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
         <v>103</v>
       </c>
@@ -12852,7 +12850,7 @@
         <v>7372.9025027751904</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
         <v>104</v>
       </c>
@@ -12860,7 +12858,7 @@
         <v>1747.8282780647301</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
         <v>105</v>
       </c>
@@ -12868,7 +12866,7 @@
         <v>8474.5299254655802</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
         <v>106</v>
       </c>
@@ -12876,7 +12874,7 @@
         <v>13995.496036768</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
         <v>107</v>
       </c>
@@ -12884,7 +12882,7 @@
         <v>16852.628568410899</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
         <v>108</v>
       </c>
@@ -12892,7 +12890,7 @@
         <v>4083.0758166313199</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">
         <v>109</v>
       </c>
@@ -12900,7 +12898,7 @@
         <v>10733.778172492999</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="11" t="s">
         <v>110</v>
       </c>
@@ -12908,7 +12906,7 @@
         <v>3896.1977550983402</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
         <v>111</v>
       </c>
@@ -12916,7 +12914,7 @@
         <v>26299.587141036998</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
         <v>112</v>
       </c>
@@ -12924,7 +12922,7 @@
         <v>23209.981265306498</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="11" t="s">
         <v>113</v>
       </c>
@@ -12932,7 +12930,7 @@
         <v>24945.959003090898</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="11" t="s">
         <v>114</v>
       </c>
@@ -12940,7 +12938,7 @@
         <v>59748.997807741202</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="11" t="s">
         <v>115</v>
       </c>
@@ -12948,7 +12946,7 @@
         <v>14393.622730732</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="19" t="s">
         <v>116</v>
       </c>
@@ -12956,7 +12954,7 @@
         <v>246937.177093148</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="11" t="s">
         <v>117</v>
       </c>
@@ -12964,7 +12962,7 @@
         <v>21276.021699428598</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="11" t="s">
         <v>118</v>
       </c>
@@ -12972,7 +12970,7 @@
         <v>34610.533058047302</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="11" t="s">
         <v>119</v>
       </c>
@@ -12980,7 +12978,7 @@
         <v>17494.728096485102</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="11" t="s">
         <v>120</v>
       </c>
@@ -12988,7 +12986,7 @@
         <v>16875.0218381882</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="11" t="s">
         <v>121</v>
       </c>
@@ -12996,7 +12994,7 @@
         <v>33075.851939916603</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="11" t="s">
         <v>122</v>
       </c>
@@ -13004,7 +13002,7 @@
         <v>13009.9575910568</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="11" t="s">
         <v>123</v>
       </c>
@@ -13012,7 +13010,7 @@
         <v>99.5713467597961</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="11" t="s">
         <v>124</v>
       </c>
@@ -13020,7 +13018,7 @@
         <v>26914.621000289899</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="11" t="s">
         <v>125</v>
       </c>
@@ -13028,7 +13026,7 @@
         <v>26348.408651113499</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="11" t="s">
         <v>126</v>
       </c>
@@ -13036,7 +13034,7 @@
         <v>22411.589735984799</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="11" t="s">
         <v>127</v>
       </c>
@@ -13044,7 +13042,7 @@
         <v>21339.225187778498</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="11" t="s">
         <v>128</v>
       </c>
@@ -13052,7 +13050,7 @@
         <v>3073.0704047679901</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="11" t="s">
         <v>129</v>
       </c>
@@ -13060,7 +13058,7 @@
         <v>3161.5227546691899</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="11" t="s">
         <v>130</v>
       </c>
@@ -13068,7 +13066,7 @@
         <v>7247.0537886619604</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="19" t="s">
         <v>131</v>
       </c>
@@ -13076,7 +13074,7 @@
         <v>150467.23000144999</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="11" t="s">
         <v>132</v>
       </c>
@@ -13084,7 +13082,7 @@
         <v>43726.817496776603</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="11" t="s">
         <v>133</v>
       </c>
@@ -13092,7 +13090,7 @@
         <v>75246.109485626206</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="11" t="s">
         <v>134</v>
       </c>
@@ -13100,7 +13098,7 @@
         <v>27183.775907516501</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="11" t="s">
         <v>135</v>
       </c>
@@ -13108,7 +13106,7 @@
         <v>2551.8674988746602</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="11" t="s">
         <v>136</v>
       </c>
@@ -13116,7 +13114,7 @@
         <v>1758.6596126556401</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="19" t="s">
         <v>137</v>
       </c>
@@ -13124,7 +13122,7 @@
         <v>17265.104497909499</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="11" t="s">
         <v>138</v>
       </c>
@@ -13132,7 +13130,7 @@
         <v>649.35433197021496</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="11" t="s">
         <v>139</v>
       </c>
@@ -13140,7 +13138,7 @@
         <v>11412.956697940799</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="11" t="s">
         <v>140</v>
       </c>
@@ -13148,7 +13146,7 @@
         <v>532.68493676185597</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="11" t="s">
         <v>141</v>
       </c>
@@ -13156,7 +13154,7 @@
         <v>1543.2159569263499</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="11" t="s">
         <v>142</v>
       </c>
@@ -13164,7 +13162,7 @@
         <v>2839.2534923553499</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="11" t="s">
         <v>143</v>
       </c>
@@ -13172,7 +13170,7 @@
         <v>287.639081954956</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="19" t="s">
         <v>144</v>
       </c>
@@ -13180,7 +13178,7 @@
         <v>11291.7082164288</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="11" t="s">
         <v>145</v>
       </c>
@@ -13188,7 +13186,7 @@
         <v>502.16327810287498</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="11" t="s">
         <v>146</v>
       </c>
@@ -13196,7 +13194,7 @@
         <v>167.48792982101401</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="11" t="s">
         <v>147</v>
       </c>
@@ -13204,7 +13202,7 @@
         <v>286.61314320564298</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="11" t="s">
         <v>148</v>
       </c>
@@ -13212,7 +13210,7 @@
         <v>378.389812707901</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="11" t="s">
         <v>149</v>
       </c>
@@ -13220,7 +13218,7 @@
         <v>458.78344011306802</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="11" t="s">
         <v>150</v>
       </c>
@@ -13228,7 +13226,7 @@
         <v>814.74685907363903</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="11" t="s">
         <v>151</v>
       </c>
@@ -13236,7 +13234,7 @@
         <v>894.272755622864</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="11" t="s">
         <v>152</v>
       </c>
@@ -13244,7 +13242,7 @@
         <v>715.97156047820999</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="11" t="s">
         <v>153</v>
       </c>
@@ -13252,7 +13250,7 @@
         <v>74.520860195159898</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="11" t="s">
         <v>154</v>
       </c>
@@ -13260,7 +13258,7 @@
         <v>958.77032423019398</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="11" t="s">
         <v>155</v>
       </c>
@@ -13268,7 +13266,7 @@
         <v>448.12758231163002</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="11" t="s">
         <v>156</v>
       </c>
@@ -13276,7 +13274,7 @@
         <v>480.99934148788498</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="23" t="s">
         <v>157</v>
       </c>
@@ -13293,23 +13291,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41A3D045-D0ED-4D2D-A162-8D04FA69768E}">
   <dimension ref="A1:B71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.15234375" customWidth="1"/>
-    <col min="2" max="2" width="13.53515625" style="49" customWidth="1"/>
+    <col min="1" max="1" width="27.1796875" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" style="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="68"/>
       <c r="B1" s="72" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
         <v>88</v>
       </c>
@@ -13317,7 +13315,7 @@
         <v>749021.96234870004</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="19" t="s">
         <v>89</v>
       </c>
@@ -13325,7 +13323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
         <v>90</v>
       </c>
@@ -13333,7 +13331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>91</v>
       </c>
@@ -13341,7 +13339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>92</v>
       </c>
@@ -13349,7 +13347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>93</v>
       </c>
@@ -13357,7 +13355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
         <v>94</v>
       </c>
@@ -13365,7 +13363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
         <v>95</v>
       </c>
@@ -13373,7 +13371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>96</v>
       </c>
@@ -13381,7 +13379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
         <v>97</v>
       </c>
@@ -13389,7 +13387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
         <v>98</v>
       </c>
@@ -13397,7 +13395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
         <v>99</v>
       </c>
@@ -13405,7 +13403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
         <v>100</v>
       </c>
@@ -13413,7 +13411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="19" t="s">
         <v>101</v>
       </c>
@@ -13421,7 +13419,7 @@
         <v>35583.749362230301</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
         <v>102</v>
       </c>
@@ -13429,7 +13427,7 @@
         <v>10.433447837829601</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
         <v>103</v>
       </c>
@@ -13437,7 +13435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
         <v>104</v>
       </c>
@@ -13445,7 +13443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
         <v>105</v>
       </c>
@@ -13453,7 +13451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
         <v>106</v>
       </c>
@@ -13461,7 +13459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
         <v>107</v>
       </c>
@@ -13469,7 +13467,7 @@
         <v>8.2964839935302699</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
         <v>108</v>
       </c>
@@ -13477,7 +13475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">
         <v>109</v>
       </c>
@@ -13485,7 +13483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="11" t="s">
         <v>110</v>
       </c>
@@ -13493,7 +13491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
         <v>111</v>
       </c>
@@ -13501,7 +13499,7 @@
         <v>8.7252931594848597</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
         <v>112</v>
       </c>
@@ -13509,7 +13507,7 @@
         <v>1695.4479434490199</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="11" t="s">
         <v>113</v>
       </c>
@@ -13517,7 +13515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="11" t="s">
         <v>114</v>
       </c>
@@ -13525,7 +13523,7 @@
         <v>33860.846193790399</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="11" t="s">
         <v>115</v>
       </c>
@@ -13533,7 +13531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="19" t="s">
         <v>116</v>
       </c>
@@ -13541,7 +13539,7 @@
         <v>8099.5470976829502</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="11" t="s">
         <v>117</v>
       </c>
@@ -13549,7 +13547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="11" t="s">
         <v>118</v>
       </c>
@@ -13557,7 +13555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="11" t="s">
         <v>119</v>
       </c>
@@ -13565,7 +13563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="11" t="s">
         <v>120</v>
       </c>
@@ -13573,7 +13571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="11" t="s">
         <v>121</v>
       </c>
@@ -13581,7 +13579,7 @@
         <v>5563.3889088630704</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="11" t="s">
         <v>122</v>
       </c>
@@ -13589,7 +13587,7 @@
         <v>29.051733970642101</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="11" t="s">
         <v>123</v>
       </c>
@@ -13597,7 +13595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="11" t="s">
         <v>124</v>
       </c>
@@ -13605,7 +13603,7 @@
         <v>8.4093303680419904</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="11" t="s">
         <v>125</v>
       </c>
@@ -13613,7 +13611,7 @@
         <v>509.14502716064499</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="11" t="s">
         <v>126</v>
       </c>
@@ -13621,7 +13619,7 @@
         <v>438.69213962554898</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="11" t="s">
         <v>127</v>
       </c>
@@ -13629,7 +13627,7 @@
         <v>175.42650079727201</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="11" t="s">
         <v>128</v>
       </c>
@@ -13637,7 +13635,7 @@
         <v>322.37047100067099</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="11" t="s">
         <v>129</v>
       </c>
@@ -13645,7 +13643,7 @@
         <v>19.744504451751698</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="11" t="s">
         <v>130</v>
       </c>
@@ -13653,7 +13651,7 @@
         <v>1033.31848144531</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="19" t="s">
         <v>131</v>
       </c>
@@ -13661,7 +13659,7 @@
         <v>685268.45528030396</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="11" t="s">
         <v>132</v>
       </c>
@@ -13669,7 +13667,7 @@
         <v>37364.040694951997</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="11" t="s">
         <v>133</v>
       </c>
@@ -13677,7 +13675,7 @@
         <v>127412.608041763</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="11" t="s">
         <v>134</v>
       </c>
@@ -13685,7 +13683,7 @@
         <v>244832.67942023301</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="11" t="s">
         <v>135</v>
       </c>
@@ -13693,7 +13691,7 @@
         <v>110936.914189816</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="11" t="s">
         <v>136</v>
       </c>
@@ -13701,7 +13699,7 @@
         <v>164722.21293353999</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="19" t="s">
         <v>137</v>
       </c>
@@ -13709,7 +13707,7 @@
         <v>20035.372874259901</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="11" t="s">
         <v>138</v>
       </c>
@@ -13717,7 +13715,7 @@
         <v>11116.280725956</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="11" t="s">
         <v>139</v>
       </c>
@@ -13725,7 +13723,7 @@
         <v>7.5587410926818803</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="11" t="s">
         <v>140</v>
       </c>
@@ -13733,7 +13731,7 @@
         <v>15.0225644111633</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="11" t="s">
         <v>141</v>
       </c>
@@ -13741,7 +13739,7 @@
         <v>6597.0553240776098</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="11" t="s">
         <v>142</v>
       </c>
@@ -13749,7 +13747,7 @@
         <v>2299.4555187225301</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="11" t="s">
         <v>143</v>
       </c>
@@ -13757,7 +13755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="19" t="s">
         <v>144</v>
       </c>
@@ -13765,7 +13763,7 @@
         <v>34.837734222412102</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="11" t="s">
         <v>145</v>
       </c>
@@ -13773,7 +13771,7 @@
         <v>34.837734222412102</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" s="11" t="s">
         <v>146</v>
       </c>
@@ -13781,7 +13779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="11" t="s">
         <v>147</v>
       </c>
@@ -13789,7 +13787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" s="11" t="s">
         <v>148</v>
       </c>
@@ -13797,7 +13795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" s="11" t="s">
         <v>149</v>
       </c>
@@ -13805,7 +13803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" s="11" t="s">
         <v>150</v>
       </c>
@@ -13813,7 +13811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="11" t="s">
         <v>151</v>
       </c>
@@ -13821,7 +13819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="11" t="s">
         <v>152</v>
       </c>
@@ -13829,7 +13827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="11" t="s">
         <v>153</v>
       </c>
@@ -13837,7 +13835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="11" t="s">
         <v>154</v>
       </c>
@@ -13845,7 +13843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" s="11" t="s">
         <v>155</v>
       </c>
@@ -13853,7 +13851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="11" t="s">
         <v>156</v>
       </c>
@@ -13861,7 +13859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" s="23" t="s">
         <v>157</v>
       </c>

</xml_diff>